<commit_message>
fixed all the issues in supplier feature and build skeleton for supermarket feature
</commit_message>
<xml_diff>
--- a/Faiqa_Yasmeen_Hetul/src/main/resources/items.xlsx
+++ b/Faiqa_Yasmeen_Hetul/src/main/resources/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HETUL\LaSalle\2nd sem\information system\assignment\assignment2\mavenProject\Faiqa_Yasmeen_Hetul\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD0F46-49ED-4D51-973F-34A437CCBC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F625D5AF-40DF-4A7F-A7AA-1C916862D9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>apple</t>
   </si>
@@ -58,6 +58,54 @@
   </si>
   <si>
     <t>shailraj bhai ni born vitta joine amne i6a thai</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>kiwi</t>
+  </si>
+  <si>
+    <t>kiwi1</t>
+  </si>
+  <si>
+    <t>sfjskls</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>bakery</t>
+  </si>
+  <si>
+    <t>fsdklffklssf</t>
+  </si>
+  <si>
+    <t>cupcake</t>
+  </si>
+  <si>
+    <t>fdsjklsdfd;lk</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>fjsdklsdjfs</t>
   </si>
 </sst>
 </file>
@@ -375,83 +423,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buying feature and display feature added in supermarket and warehouse class created with required attributes and method
</commit_message>
<xml_diff>
--- a/Faiqa_Yasmeen_Hetul/src/main/resources/items.xlsx
+++ b/Faiqa_Yasmeen_Hetul/src/main/resources/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HETUL\LaSalle\2nd sem\information system\assignment\assignment2\mavenProject\Faiqa_Yasmeen_Hetul\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F625D5AF-40DF-4A7F-A7AA-1C916862D9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7A06A3-27CA-4FC2-B2F3-B3A993AE43E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>apple</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>fjsdklsdjfs</t>
+  </si>
+  <si>
+    <t>apple2</t>
+  </si>
+  <si>
+    <t>oyeoyeoye</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,6 +605,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>